<commit_message>
modified init files to add more scenarios
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E45B7B-A643-4B5E-A0CC-5A50D4116B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8904BB5A-98A0-425C-A3A6-C429F2EB54BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -234,25 +235,25 @@
     <t>O475</t>
   </si>
   <si>
-    <t>A36</t>
-  </si>
-  <si>
-    <t>B36</t>
-  </si>
-  <si>
-    <t>C36</t>
-  </si>
-  <si>
-    <t>G36</t>
-  </si>
-  <si>
-    <t>H36</t>
-  </si>
-  <si>
-    <t>I36</t>
-  </si>
-  <si>
-    <t>J36</t>
+    <t>A39</t>
+  </si>
+  <si>
+    <t>B39</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>G39</t>
+  </si>
+  <si>
+    <t>H39</t>
+  </si>
+  <si>
+    <t>I39</t>
+  </si>
+  <si>
+    <t>J39</t>
   </si>
 </sst>
 </file>

</xml_diff>